<commit_message>
adding a file for the nutrient solution
</commit_message>
<xml_diff>
--- a/manuscript/Figures_&_tables/Supplementary Table 3 Nutrient Solution.xlsx
+++ b/manuscript/Figures_&_tables/Supplementary Table 3 Nutrient Solution.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\montazeaud\Documents\RECHERCHE\Postdoc\Montpellier\SolACE 3\SolACE_wheat_mixtures\manuscript\Figures_&amp;_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7B24BA8A-8FFB-41A1-8344-0B8C0867CEFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{633C17C1-B48A-4731-9FF9-E8479E5B1D04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{9AEEB456-9BA0-4284-ADCD-FE894DC80AAE}"/>
   </bookViews>
@@ -150,17 +150,17 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -478,8 +478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67C84A69-4DDC-479A-9802-2E9714D35626}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -490,34 +490,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
     </row>
     <row r="3" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -575,11 +575,11 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
@@ -648,9 +648,10 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="A1:C2"/>
+    <mergeCell ref="A10:C10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>